<commit_message>
i have update the logout method
</commit_message>
<xml_diff>
--- a/AK_CORE/xls/RegressionSuite.xlsx
+++ b/AK_CORE/xls/RegressionSuite.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226" filterPrivacy="1"/>
+  <xr:revisionPtr documentId="13_ncr:1_{BD772D78-73C6-49D2-A47A-26BC2F72B953}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="6825" windowWidth="11280" xWindow="240" yWindow="105"/>
+    <workbookView activeTab="2" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" r:id="rId1" sheetId="3"/>
-    <sheet name="TestCase1" r:id="rId2" sheetId="15"/>
+    <sheet name="TestCase2" r:id="rId2" sheetId="16"/>
+    <sheet name="TestCase1" r:id="rId3" sheetId="15"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>TCID</t>
   </si>
@@ -48,12 +50,36 @@
   </si>
   <si>
     <t>Errors</t>
+  </si>
+  <si>
+    <t>TestCase2</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>TestCase3</t>
+  </si>
+  <si>
+    <t>Logout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -95,7 +121,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,6 +157,21 @@
       </patternFill>
     </fill>
     <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
       <patternFill patternType="none">
         <fgColor indexed="17"/>
       </patternFill>
@@ -190,8 +231,18 @@
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -230,6 +281,69 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <bottom style="thick"/>
+    </border>
+    <border>
+      <top style="thick"/>
+      <bottom style="thick"/>
+    </border>
+    <border>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
+    </border>
+    <border>
+      <left style="thick"/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
+    </border>
+    <border>
       <bottom style="thick"/>
     </border>
     <border>
@@ -344,28 +458,31 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="6" fillId="8" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="10" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="14" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="18" fillId="14" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="22" fillId="16" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="26" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="1" applyFill="1" borderId="2" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="3" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="4" fillId="8" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="5" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="9" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="13" fillId="13" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="15" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="21" fillId="17" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="25" fillId="19" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="29" fillId="21" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="33" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle name="Hyperlink 2" xfId="3"/>
+    <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -700,23 +817,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="35.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="56.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="35.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="56.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="9.72265625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="18.75" r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row ht="18" r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,71 +847,166 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="90" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="90"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;LUnrestricted </oddFooter>
+    <evenFooter xml:space="preserve">&amp;LUnrestricted </evenFooter>
+    <firstFooter xml:space="preserve">&amp;LUnrestricted </firstFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05DA9BA-278B-4456-8C59-7D8683C61749}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;LUnrestricted </oddFooter>
+    <evenFooter xml:space="preserve">&amp;LUnrestricted </evenFooter>
+    <firstFooter xml:space="preserve">&amp;LUnrestricted </firstFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.640625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="25.5546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="16.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2"/>
+    <hyperlink r:id="rId1" ref="A2" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;LUnrestricted </oddFooter>
+    <evenFooter xml:space="preserve">&amp;LUnrestricted </evenFooter>
+    <firstFooter xml:space="preserve">&amp;LUnrestricted </firstFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>